<commit_message>
added usecases to sprint plan
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htlgrieskirchenat-my.sharepoint.com/personal/kaliuzhnyiv190154_sus_htl-grieskirchen_at/Documents/2023-24/SYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vadym2005/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A247A12-6203-0A4A-B4CD-588824439C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F55DA2-EDE0-1C4D-9F2E-21088B027214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F3D3D1BE-4D88-D641-A187-67C9CB798FC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Zeitraum des Sprints</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Graf anzeigen</t>
+  </si>
+  <si>
+    <t>Passwort für Zielsetzung</t>
+  </si>
+  <si>
+    <t>Ansichtwechsel Admin App</t>
+  </si>
+  <si>
+    <t>Passwort für Zurücksetzen</t>
   </si>
 </sst>
 </file>
@@ -111,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +145,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -192,37 +207,39 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -539,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98256B98-E916-B346-BDDE-9673E69755D9}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,149 +574,195 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="6">
         <v>1</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="9">
+      <c r="C1" s="7"/>
+      <c r="D1" s="6">
         <v>2</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="9">
+      <c r="E1" s="7"/>
+      <c r="F1" s="6">
         <v>3</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="9">
+      <c r="G1" s="7"/>
+      <c r="H1" s="6">
         <v>4</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="9">
+      <c r="I1" s="7"/>
+      <c r="J1" s="6">
         <v>5</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="9">
+      <c r="K1" s="7"/>
+      <c r="L1" s="6">
         <v>6</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="9">
+      <c r="M1" s="7"/>
+      <c r="N1" s="6">
         <v>7</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="9">
+      <c r="O1" s="7"/>
+      <c r="P1" s="6">
         <v>8</v>
       </c>
-      <c r="Q1" s="10"/>
+      <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="7" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="7" t="s">
+      <c r="M2" s="5"/>
+      <c r="N2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="7" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="8"/>
+      <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="13"/>
+      <c r="J3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
     </row>
-    <row r="5" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="44">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="L2:M2"/>
@@ -710,37 +773,12 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added content to excel and docx
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vadym2005/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HtlFolder\4Klasse\SYP\SYP-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7C7B0C-DA08-8D47-8F67-17D60AA47020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3775796-1B63-45F5-872B-C4B4F0C57D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F3D3D1BE-4D88-D641-A187-67C9CB798FC7}"/>
+    <workbookView xWindow="2670" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{F3D3D1BE-4D88-D641-A187-67C9CB798FC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Zeitraum des Sprints</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>Zielsetzung bestätigen</t>
+  </si>
+  <si>
+    <t>Bericht versenden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisierung </t>
+  </si>
+  <si>
+    <t>Anordnung von Maschinen endern</t>
   </si>
 </sst>
 </file>
@@ -217,22 +226,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -242,22 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,177 +580,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98256B98-E916-B346-BDDE-9673E69755D9}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="8">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="5">
+      <c r="C1" s="9"/>
+      <c r="D1" s="8">
         <v>2</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5">
+      <c r="E1" s="9"/>
+      <c r="F1" s="8">
         <v>3</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="5">
+      <c r="G1" s="9"/>
+      <c r="H1" s="8">
         <v>4</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="5">
+      <c r="I1" s="9"/>
+      <c r="J1" s="8">
         <v>5</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="5">
+      <c r="K1" s="9"/>
+      <c r="L1" s="8">
         <v>6</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="5">
+      <c r="M1" s="9"/>
+      <c r="N1" s="8">
         <v>7</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="5">
+      <c r="O1" s="9"/>
+      <c r="P1" s="8">
         <v>8</v>
       </c>
-      <c r="Q1" s="6"/>
+      <c r="Q1" s="9"/>
     </row>
-    <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="10" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="10" t="s">
+      <c r="M2" s="5"/>
+      <c r="N2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="10" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="11"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="3">
+        <v>45394</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4" t="s">
+      <c r="M3" s="10"/>
+      <c r="N3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="7" t="s">
+      <c r="O3" s="10"/>
+      <c r="P3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="7"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="L4" s="4" t="s">
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="L4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="14" t="s">
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="14"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7" t="s">
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="7"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="L2:M2"/>
@@ -759,31 +801,8 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="P4:Q4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>